<commit_message>
Added files for class.
</commit_message>
<xml_diff>
--- a/Sessions/I/Activities/006-Student-LineCharts/Unsolved/StudentAvgScores.xlsx
+++ b/Sessions/I/Activities/006-Student-LineCharts/Unsolved/StudentAvgScores.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paularias/Documents/EPIC Journey to Professional Careers/DataVisualization-Curriculum/Sessions/I/Activities/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paularias/Documents/EPIC Journey to Professional Careers/DataVisualization-Curriculum/Sessions/I/Activities/006-Student-LineCharts/Unsolved/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C19158A-A7D5-6249-8AC3-748550760309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{527C76C8-59C6-274D-84CD-4C468021795B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6460" yWindow="3800" windowWidth="28040" windowHeight="17440" xr2:uid="{DA27FCC0-D5C6-E748-BB73-D15F564283F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -469,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{144F9D8D-B8E6-F645-9E65-3999BFC73A17}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>